<commit_message>
Update Hiawatha and OttawaNF scripts
</commit_message>
<xml_diff>
--- a/lookupTables/behavior.xlsx
+++ b/lookupTables/behavior.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MelinaStuff\BAM\WildTrax\WT-Integration\lookupTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A84617-3C6B-4DBF-BB35-19FCA68D3DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A49EA16-EAF2-4295-AEBD-A1A8B1549FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="80">
   <si>
     <t>BEHAVIOURID</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes / No / DNC </t>
+  </si>
+  <si>
+    <t>Male / Female</t>
   </si>
 </sst>
 </file>
@@ -717,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +792,7 @@
         <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>60</v>
@@ -859,7 +862,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>70</v>
       </c>

</xml_diff>